<commit_message>
fourniture des fichiers xlsx pour les documents liés à une entreprise
</commit_message>
<xml_diff>
--- a/impact/analyseia/xlsx/template_synthese_ESG.xlsx
+++ b/impact/analyseia/xlsx/template_synthese_ESG.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t xml:space="preserve">Synthèse générique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thème</t>
   </si>
   <si>
     <t xml:space="preserve">Fichier</t>
@@ -133,7 +136,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -146,6 +149,13 @@
       <right style="medium"/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right/>
+      <top style="medium"/>
+      <bottom style="medium"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -188,7 +198,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -209,19 +219,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -318,7 +332,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Image 1" descr="Logo-Ministère-de-l'économie-et-des-finances-(2020) - EXAG"/>
+        <xdr:cNvPr id="1" name="Image 1" descr="Logo-Ministère-de-l'économie-et-des-finances-(2020) - EXAG"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -327,7 +341,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="976680" y="571680"/>
+          <a:off x="1231920" y="571680"/>
           <a:ext cx="1367640" cy="977400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -356,7 +370,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Image 2" descr=""/>
+        <xdr:cNvPr id="2" name="Image 2" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -365,8 +379,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10158840" y="571680"/>
-          <a:ext cx="1196280" cy="951840"/>
+          <a:off x="12814200" y="571680"/>
+          <a:ext cx="1396440" cy="951840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -563,15 +577,15 @@
   <dimension ref="C10:K31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.85"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="1" width="10.85"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="1" width="10.86"/>
   </cols>
   <sheetData>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -619,34 +633,36 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="11.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="11.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="11.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="6" width="11.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16383" min="7" style="6" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="6" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="11.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="5" width="11.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="D1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>